<commit_message>
veedoc add appointment page
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umairasif/git/repository/IOS/VeeDoc_AndroidTest/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7157C8E1-E7B4-E14A-89CE-A6F439C2C53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBB2B6D-8353-4E43-9C31-5BBCCB532F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{3C9FE245-85DA-4214-BC29-FC8BCB191588}"/>
+    <workbookView xWindow="31980" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{3C9FE245-85DA-4214-BC29-FC8BCB191588}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="profile" sheetId="2" r:id="rId2"/>
+    <sheet name="quickappointment" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Email</t>
   </si>
@@ -90,6 +91,24 @@
   </si>
   <si>
     <t>Bhutto, A</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>timezone</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>Test data input</t>
+  </si>
+  <si>
+    <t>Asghar</t>
   </si>
 </sst>
 </file>
@@ -461,7 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84AFC031-54B8-48BB-9B24-B085B0F11A87}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -507,7 +526,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -574,4 +593,65 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CEEEEF-39F7-9947-A1C5-115F621857E7}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3162833883</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{58CB32AE-C0D2-954F-B671-6A71184FB6C0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>